<commit_message>
Fixed a small typo in the raw data and did posthoc analyses for female experiment for number of inseminations.
</commit_message>
<xml_diff>
--- a/females/data/raw/fem_summary_data.xlsx
+++ b/females/data/raw/fem_summary_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janya\Desktop\R\bb_soc_exp\females\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jy33\OneDrive\Desktop\R\bb_soc_exp\females\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92B5E1D-7CBB-4210-B81E-2CFAB4E6A7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32894BC-63D8-41AC-8F72-2878E360A265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="75" yWindow="368" windowWidth="20445" windowHeight="12914" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -465,24 +465,24 @@
   <dimension ref="A1:L145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.86328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.73046875" customWidth="1"/>
+    <col min="4" max="4" width="10.86328125" customWidth="1"/>
+    <col min="5" max="5" width="14.86328125" customWidth="1"/>
+    <col min="7" max="7" width="16.1328125" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.1328125" customWidth="1"/>
+    <col min="10" max="10" width="14.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -520,7 +520,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -554,7 +554,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -588,7 +588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -622,7 +622,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -656,7 +656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -690,7 +690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -724,7 +724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>1</v>
       </c>
@@ -758,7 +758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -791,7 +791,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>1</v>
       </c>
@@ -825,7 +825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>1</v>
       </c>
@@ -859,7 +859,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>1</v>
       </c>
@@ -893,7 +893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>1</v>
       </c>
@@ -927,7 +927,7 @@
         <v>0.77777777777777779</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <v>1</v>
       </c>
@@ -961,7 +961,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <v>1</v>
       </c>
@@ -994,7 +994,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <v>1</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <v>1</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <v>1</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <v>1</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <v>1</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <v>1</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <v>1</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <v>1</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <v>1</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <v>1</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <v>2</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <v>2</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <v>2</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <v>2</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <v>2</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <v>2</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
         <v>2</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="2">
         <v>2</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>0.52173913043478259</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="2">
         <v>2</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" s="2">
         <v>2</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="2">
         <v>2</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="2">
         <v>2</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="2">
         <v>2</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="2">
         <v>2</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>0.45454545454545453</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="2">
         <v>2</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="2">
         <v>2</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>0.54545454545454541</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" s="2">
         <v>2</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" s="2">
         <v>2</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>0.65217391304347827</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" s="2">
         <v>2</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" s="2">
         <v>2</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" s="2">
         <v>2</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" s="2">
         <v>2</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" s="2">
         <v>2</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A49" s="2">
         <v>2</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A50" s="2">
         <v>4</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A51" s="2">
         <v>4</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A52" s="2">
         <v>4</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A53" s="2">
         <v>4</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A54" s="2">
         <v>4</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A55" s="2">
         <v>4</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A56" s="2">
         <v>4</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A57" s="2">
         <v>4</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>0.72727272727272729</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A58" s="2">
         <v>4</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>0.7857142857142857</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A59" s="2">
         <v>4</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A60" s="2">
         <v>4</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A61" s="2">
         <v>4</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>0.8571428571428571</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A62" s="2">
         <v>4</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A63" s="2">
         <v>4</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A64" s="2">
         <v>4</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65" s="2">
         <v>4</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66" s="2">
         <v>4</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A67" s="2">
         <v>4</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A68" s="2">
         <v>4</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A69" s="2">
         <v>4</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A70" s="2">
         <v>4</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>0.77777777777777779</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A71" s="2">
         <v>4</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72" s="2">
         <v>4</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73" s="2">
         <v>4</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A74" s="2">
         <v>3</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A75" s="2">
         <v>3</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A76" s="2">
         <v>3</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A77" s="2">
         <v>3</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A78" s="2">
         <v>3</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A79" s="2">
         <v>3</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A80" s="2">
         <v>3</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A81" s="2">
         <v>3</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A82" s="2">
         <v>3</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>0.14285714285714285</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A83" s="2">
         <v>3</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A84" s="2">
         <v>3</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A85" s="2">
         <v>3</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A86" s="2">
         <v>3</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A87" s="2">
         <v>3</v>
       </c>
@@ -3445,7 +3445,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A88" s="2">
         <v>3</v>
       </c>
@@ -3479,7 +3479,7 @@
         <v>0.7142857142857143</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A89" s="2">
         <v>3</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>0.84210526315789469</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A90" s="2">
         <v>3</v>
       </c>
@@ -3547,7 +3547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A91" s="2">
         <v>3</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>0.91428571428571426</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A92" s="2">
         <v>3</v>
       </c>
@@ -3615,7 +3615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A93" s="2">
         <v>3</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A94" s="2">
         <v>3</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v>0.93548387096774188</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A95" s="2">
         <v>3</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>0.7142857142857143</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A96" s="2">
         <v>3</v>
       </c>
@@ -3750,7 +3750,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A97" s="2">
         <v>3</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>0.7142857142857143</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A98" s="2">
         <v>5</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A99" s="2">
         <v>5</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A100" s="2">
         <v>5</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A101" s="2">
         <v>5</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A102" s="2">
         <v>5</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>12</v>
       </c>
       <c r="E102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F102">
         <v>2</v>
@@ -3954,7 +3954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A103" s="2">
         <v>5</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A104" s="2">
         <v>5</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A105" s="2">
         <v>5</v>
       </c>
@@ -4056,7 +4056,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A106" s="2">
         <v>5</v>
       </c>
@@ -4090,7 +4090,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A107" s="2">
         <v>5</v>
       </c>
@@ -4124,7 +4124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A108" s="2">
         <v>5</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A109" s="2">
         <v>5</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A110" s="2">
         <v>5</v>
       </c>
@@ -4226,7 +4226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A111" s="2">
         <v>5</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A112" s="2">
         <v>5</v>
       </c>
@@ -4294,7 +4294,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A113" s="2">
         <v>5</v>
       </c>
@@ -4328,7 +4328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A114" s="2">
         <v>5</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A115" s="2">
         <v>5</v>
       </c>
@@ -4396,7 +4396,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A116" s="2">
         <v>5</v>
       </c>
@@ -4430,7 +4430,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A117" s="2">
         <v>5</v>
       </c>
@@ -4464,7 +4464,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A118" s="2">
         <v>5</v>
       </c>
@@ -4498,7 +4498,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A119" s="2">
         <v>5</v>
       </c>
@@ -4532,7 +4532,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A120" s="2">
         <v>5</v>
       </c>
@@ -4566,7 +4566,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A121" s="2">
         <v>5</v>
       </c>
@@ -4600,7 +4600,7 @@
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A122" s="2">
         <v>6</v>
       </c>
@@ -4634,7 +4634,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A123" s="2">
         <v>6</v>
       </c>
@@ -4668,7 +4668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A124" s="2">
         <v>6</v>
       </c>
@@ -4708,7 +4708,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A125" s="2">
         <v>6</v>
       </c>
@@ -4742,7 +4742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A126" s="2">
         <v>6</v>
       </c>
@@ -4776,7 +4776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A127" s="2">
         <v>6</v>
       </c>
@@ -4816,7 +4816,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A128" s="2">
         <v>6</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A129" s="2">
         <v>6</v>
       </c>
@@ -4884,7 +4884,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A130" s="2">
         <v>6</v>
       </c>
@@ -4924,7 +4924,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A131" s="2">
         <v>6</v>
       </c>
@@ -4957,7 +4957,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A132" s="2">
         <v>6</v>
       </c>
@@ -4991,7 +4991,7 @@
         <v>0.8571428571428571</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A133" s="2">
         <v>6</v>
       </c>
@@ -5031,7 +5031,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A134" s="2">
         <v>6</v>
       </c>
@@ -5064,7 +5064,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A135" s="2">
         <v>6</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A136" s="2">
         <v>6</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A137" s="2">
         <v>6</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A138" s="2">
         <v>6</v>
       </c>
@@ -5206,7 +5206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A139" s="2">
         <v>6</v>
       </c>
@@ -5246,7 +5246,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A140" s="2">
         <v>6</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A141" s="2">
         <v>6</v>
       </c>
@@ -5314,7 +5314,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A142" s="2">
         <v>6</v>
       </c>
@@ -5354,7 +5354,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A143" s="2">
         <v>6</v>
       </c>
@@ -5388,7 +5388,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A144" s="2">
         <v>6</v>
       </c>
@@ -5422,7 +5422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A145" s="2">
         <v>6</v>
       </c>

</xml_diff>